<commit_message>
Add admin screen in client
</commit_message>
<xml_diff>
--- a/protocole.xlsx
+++ b/protocole.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexg\source\repos\TacticalWar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19AFDAA-4D35-4B41-A42E-E9667B1409B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3878538F-1139-4BFA-B4C5-F991631CC5AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="32">
   <si>
     <t>Source</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>Informe le client que son login/password est incorrect</t>
+  </si>
+  <si>
+    <t>AD</t>
+  </si>
+  <si>
+    <t>Envoi le client vers l'écran du mode admin</t>
   </si>
 </sst>
 </file>
@@ -473,7 +479,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:E1"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,11 +669,19 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>

</xml_diff>

<commit_message>
Implement match creation on serverside
</commit_message>
<xml_diff>
--- a/protocole.xlsx
+++ b/protocole.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexg\source\repos\TacticalWar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3878538F-1139-4BFA-B4C5-F991631CC5AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A0C235-BE9B-4E81-A3DA-16007088BC15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17940" yWindow="3975" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="46">
   <si>
     <t>Source</t>
   </si>
@@ -124,6 +124,48 @@
   </si>
   <si>
     <t>Envoi le client vers l'écran du mode admin</t>
+  </si>
+  <si>
+    <t>TL</t>
+  </si>
+  <si>
+    <t>Demande la liste des teams disponibles pour un match</t>
+  </si>
+  <si>
+    <t>Envoi la liste des équipes disponibles pour un match</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>Demande la création d'un match</t>
+  </si>
+  <si>
+    <t>matchName;idEquipe1;idEquipe2</t>
+  </si>
+  <si>
+    <t>CF</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>Informe que le match a bien été créé.</t>
+  </si>
+  <si>
+    <t>Informe que la création de match a échouée car les id d'équipe sont identiques.</t>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t>Informe que le match ne peut pas etre cree car au moins une des deux équipes a déjà un match planifié.</t>
+  </si>
+  <si>
+    <t>HW</t>
+  </si>
+  <si>
+    <t>Envoi le client vers l'écran d'attente d'un match.</t>
   </si>
 </sst>
 </file>
@@ -479,7 +521,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,54 +725,114 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="A15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+      <c r="E16" s="3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+      <c r="A17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="E17" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
+      <c r="E18" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="A19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
+      <c r="E19" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>

</xml_diff>

<commit_message>
Matchmaking integration (administrator interface)
</commit_message>
<xml_diff>
--- a/protocole.xlsx
+++ b/protocole.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexg\source\repos\TacticalWar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A0C235-BE9B-4E81-A3DA-16007088BC15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D6B2BD-15E5-4A47-BCBA-3D1284F90F83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17940" yWindow="3975" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10845" yWindow="2595" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="49">
   <si>
     <t>Source</t>
   </si>
@@ -166,6 +166,15 @@
   </si>
   <si>
     <t>Envoi le client vers l'écran d'attente d'un match.</t>
+  </si>
+  <si>
+    <t>MC</t>
+  </si>
+  <si>
+    <t>Envoi la liste des matchs planifiés et en cours (interface admin)</t>
+  </si>
+  <si>
+    <t>Demande de la liste des matchs créés (planifiés et en cours) (interface admin)</t>
   </si>
 </sst>
 </file>
@@ -520,8 +529,8 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,19 +843,37 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
+      <c r="E20" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>

</xml_diff>

<commit_message>
Add the class choice lock system (server side)
</commit_message>
<xml_diff>
--- a/protocole.xlsx
+++ b/protocole.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexg\source\repos\TacticalWar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D6B2BD-15E5-4A47-BCBA-3D1284F90F83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A726A6-81E7-4E7D-B1B6-79E67E932A88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10845" yWindow="2595" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12435" yWindow="900" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="54">
   <si>
     <t>Source</t>
   </si>
@@ -175,6 +175,21 @@
   </si>
   <si>
     <t>Demande de la liste des matchs créés (planifiés et en cours) (interface admin)</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>idClasseChoisie</t>
+  </si>
+  <si>
+    <t>Le client vérouille son choix de classe.</t>
+  </si>
+  <si>
+    <t>PO</t>
+  </si>
+  <si>
+    <t>Indique au client que son choix de classe est vérrouillé (aucune erreur n'est survenue lors de la génération automatique du placement de départ)</t>
   </si>
 </sst>
 </file>
@@ -529,8 +544,8 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,18 +891,36 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
+      <c r="A22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
+      <c r="E23" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>

</xml_diff>

<commit_message>
Add a lock choice button on ClassSelectionScreen
</commit_message>
<xml_diff>
--- a/protocole.xlsx
+++ b/protocole.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexg\source\repos\TacticalWar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A726A6-81E7-4E7D-B1B6-79E67E932A88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB035BBE-1A71-4115-A35F-199F1731861D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12435" yWindow="900" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4890" yWindow="585" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="54">
   <si>
     <t>Source</t>
   </si>
@@ -544,8 +544,8 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -917,7 +917,9 @@
       <c r="C23" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="E23" s="3" t="s">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
Begins preparation phase implementation (client & server side)
</commit_message>
<xml_diff>
--- a/protocole.xlsx
+++ b/protocole.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexg\source\repos\TacticalWar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB035BBE-1A71-4115-A35F-199F1731861D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1782D40-76E7-4E0F-8548-DC44775A564A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4890" yWindow="585" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="66">
   <si>
     <t>Source</t>
   </si>
@@ -190,6 +190,42 @@
   </si>
   <si>
     <t>Indique au client que son choix de classe est vérrouillé (aucune erreur n'est survenue lors de la génération automatique du placement de départ)</t>
+  </si>
+  <si>
+    <t>BS</t>
+  </si>
+  <si>
+    <t>battleState</t>
+  </si>
+  <si>
+    <t>Indique au client que l'état du combat a changé (phase préparation, phase combat, etc…)</t>
+  </si>
+  <si>
+    <t>Cs</t>
+  </si>
+  <si>
+    <t>Indique au client l'état prêt/pas prêt d'un personnage</t>
+  </si>
+  <si>
+    <t>idPerso;[1 ou 0]</t>
+  </si>
+  <si>
+    <t>Indique au serveur que la position est verrouillée (joueur prêt à commencer le combat)</t>
+  </si>
+  <si>
+    <t>CP</t>
+  </si>
+  <si>
+    <t>cellX;cellY</t>
+  </si>
+  <si>
+    <t>Demande un changement de position de départ au serveur</t>
+  </si>
+  <si>
+    <t>idPerso;cellX;cellY</t>
+  </si>
+  <si>
+    <t>Indique un changement de position du personnage (position de départ ou téléportation en combat)</t>
   </si>
 </sst>
 </file>
@@ -544,8 +580,8 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,40 +960,88 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
+      <c r="E26" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>

</xml_diff>

<commit_message>
Enter in battle phase when all player are ready
</commit_message>
<xml_diff>
--- a/protocole.xlsx
+++ b/protocole.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexg\source\repos\TacticalWar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TacticalWar\TacticalWar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1782D40-76E7-4E0F-8548-DC44775A564A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4890" yWindow="585" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4890" yWindow="585" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="68">
   <si>
     <t>Source</t>
   </si>
@@ -226,12 +225,18 @@
   </si>
   <si>
     <t>Indique un changement de position du personnage (position de départ ou téléportation en combat)</t>
+  </si>
+  <si>
+    <t>Ct</t>
+  </si>
+  <si>
+    <t>Indique au client le début du tour du joueur.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -576,12 +581,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
+      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1044,11 +1049,21 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
+      <c r="A29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
@@ -1156,7 +1171,7 @@
       <c r="E44" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E11" xr:uid="{E6220A88-8567-4A6B-9E50-FCAAA9B8B23C}"/>
+  <autoFilter ref="A1:E11"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Begins network move implementation
</commit_message>
<xml_diff>
--- a/protocole.xlsx
+++ b/protocole.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TacticalWar\TacticalWar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexg\source\repos\TacticalWar\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3F7188-7252-48AB-B57C-793CEEA449BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4890" yWindow="585" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="4890" yWindow="585" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="73">
   <si>
     <t>Source</t>
   </si>
@@ -231,12 +232,27 @@
   </si>
   <si>
     <t>Indique au client le début du tour du joueur.</t>
+  </si>
+  <si>
+    <t>Cm</t>
+  </si>
+  <si>
+    <t>path …</t>
+  </si>
+  <si>
+    <t>Le client indique qu'il veut se déplacer.</t>
+  </si>
+  <si>
+    <t>idPerso;path</t>
+  </si>
+  <si>
+    <t>Le serveur indique qu'un personnage se déplace.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -581,12 +597,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1066,18 +1082,38 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
+      <c r="A30" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
+      <c r="A31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
@@ -1171,7 +1207,7 @@
       <c r="E44" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E11"/>
+  <autoFilter ref="A1:E11" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Begins turn by turn battle system implementation & implements battle movement (+ resync on reconnection)
</commit_message>
<xml_diff>
--- a/protocole.xlsx
+++ b/protocole.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexg\source\repos\TacticalWar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3F7188-7252-48AB-B57C-793CEEA449BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85272642-8A64-4C83-AE49-9ED64E262C22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4890" yWindow="585" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="77">
   <si>
     <t>Source</t>
   </si>
@@ -247,6 +247,18 @@
   </si>
   <si>
     <t>Le serveur indique qu'un personnage se déplace.</t>
+  </si>
+  <si>
+    <t>Le client indique qu'il a terminé son tour de jeu.</t>
+  </si>
+  <si>
+    <t>Cp</t>
+  </si>
+  <si>
+    <t>idPerso;nbPM</t>
+  </si>
+  <si>
+    <t>Le serveur envoi l'information du nombre de PM restant du personnage actif (synchronisation quand il y a connexion en cours de combat)</t>
   </si>
 </sst>
 </file>
@@ -598,11 +610,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1089,45 +1101,63 @@
         <v>6</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>69</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="D30" s="3"/>
       <c r="E30" s="3" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>68</v>
       </c>
       <c r="D31" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E32" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
+    <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
@@ -1206,6 +1236,13 @@
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
     </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E11" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Improve UI & add launch spell implementation (still need to implement attacks effects)
</commit_message>
<xml_diff>
--- a/protocole.xlsx
+++ b/protocole.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexg\source\repos\TacticalWar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85272642-8A64-4C83-AE49-9ED64E262C22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5BE87F-9966-4A0D-A92A-F4C04D70872C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4890" yWindow="585" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="85">
   <si>
     <t>Source</t>
   </si>
@@ -259,6 +259,30 @@
   </si>
   <si>
     <t>Le serveur envoi l'information du nombre de PM restant du personnage actif (synchronisation quand il y a connexion en cours de combat)</t>
+  </si>
+  <si>
+    <t>idSpell;cellX;cellY</t>
+  </si>
+  <si>
+    <t>Le client indique qu'il veut lancer un sort.</t>
+  </si>
+  <si>
+    <t>idPerso;idSpell;cellX;cellY</t>
+  </si>
+  <si>
+    <t>Le serveur indique qu'un personnage lance un sort.</t>
+  </si>
+  <si>
+    <t>Ca</t>
+  </si>
+  <si>
+    <t>idPerso;nbPA</t>
+  </si>
+  <si>
+    <t>Le serveur envoi l'information du nombre de PA restant du personnage actif (synchronisation quand il y a connexion en cours de combat)</t>
+  </si>
+  <si>
+    <t>CL</t>
   </si>
 </sst>
 </file>
@@ -613,8 +637,8 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1160,25 +1184,55 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
+      <c r="A34" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>

</xml_diff>

<commit_message>
Add test damage in spell
</commit_message>
<xml_diff>
--- a/protocole.xlsx
+++ b/protocole.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexg\source\repos\TacticalWar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5BE87F-9966-4A0D-A92A-F4C04D70872C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8F513F-23BC-46FB-B3CE-943E417405D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4890" yWindow="585" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="88">
   <si>
     <t>Source</t>
   </si>
@@ -283,6 +283,15 @@
   </si>
   <si>
     <t>CL</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>idWinnerTeam</t>
+  </si>
+  <si>
+    <t>Le serveur indique qu'une équipe a gagné.</t>
   </si>
 </sst>
 </file>
@@ -638,7 +647,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
+      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1235,11 +1244,21 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
+      <c r="A37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>

</xml_diff>

<commit_message>
Add finished matchs list in admin mode (to get matchs results)
</commit_message>
<xml_diff>
--- a/protocole.xlsx
+++ b/protocole.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexg\source\repos\TacticalWar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8F513F-23BC-46FB-B3CE-943E417405D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6628DFB-39B0-4C84-A7B8-9A4FE2C2685A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4890" yWindow="585" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="90">
   <si>
     <t>Source</t>
   </si>
@@ -292,6 +292,12 @@
   </si>
   <si>
     <t>Le serveur indique qu'une équipe a gagné.</t>
+  </si>
+  <si>
+    <t>MF</t>
+  </si>
+  <si>
+    <t>Envoi la liste des matchs terminés (interface admin)</t>
   </si>
 </sst>
 </file>
@@ -643,11 +649,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,55 +998,55 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>50</v>
       </c>
       <c r="E23" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1051,28 +1057,30 @@
         <v>5</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D26" s="3"/>
+      <c r="D26" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="E26" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1083,62 +1091,62 @@
         <v>6</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>62</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="D27" s="3"/>
       <c r="E27" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D28" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E29" s="3" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D30" s="3"/>
+      <c r="D30" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="E30" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1149,123 +1157,131 @@
         <v>6</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>69</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="D31" s="3"/>
       <c r="E31" s="3" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>68</v>
       </c>
       <c r="D32" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E33" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="2" t="s">
+    <row r="34" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D34" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E34" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>84</v>
       </c>
       <c r="D35" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E36" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="2" t="s">
+    <row r="37" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D37" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E37" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" s="2" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D38" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E38" s="3" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
@@ -1316,6 +1332,13 @@
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
     </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E11" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>